<commit_message>
Updated random username generation.
</commit_message>
<xml_diff>
--- a/InstaBot/accounts.xlsx
+++ b/InstaBot/accounts.xlsx
@@ -356,10 +356,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -939,6 +939,160 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>kole_warren_arjun191@protonmail.com</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arjun Warren Kole </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>kole_warren_arjun191</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TqoVitqiYze</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>levi_elisha_tony387@gmail.com</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tony Elisha Levi </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>levi_elisha_tony387</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>7GYKCz$dl</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>julian_gunner_cooper673@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cooper Gunner Julian </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>julian_gunner_cooper673</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>DXGkQ*!yRo</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>sean_dash_kasen279@inbox.com</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kasen Dash Sean </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sean_dash_kasen279</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>aitmjNs)QM0</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>isaias_elijah_moises979@yahoo.com</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moises Elijah Isaias </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>isaias_elijah_moises979</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>5SVq@wKz2Al</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>eli_terry_graham532@hotmail.com</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Graham Terry Eli </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>eli_terry_graham532</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>kdJp2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>matthew_gibson_nolan260@inbox.com</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nolan Gibson Matthew </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>matthew_gibson_nolan260</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>UCvIH*LH6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>